<commit_message>
Signed-off-by: Raymond Yang <raymond.yang@mail.mcgill.ca>
</commit_message>
<xml_diff>
--- a/Data/SMD_Inventory_20200318.xlsx
+++ b/Data/SMD_Inventory_20200318.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="356">
   <si>
     <t>Category</t>
   </si>
@@ -555,6 +555,9 @@
     <t>SS-12D11G5R</t>
   </si>
   <si>
+    <t>TPS7A8500RGRT</t>
+  </si>
+  <si>
     <t>Manufacturer</t>
   </si>
   <si>
@@ -783,6 +786,9 @@
     <t>SMD,7.3x6.8x3mm</t>
   </si>
   <si>
+    <t>20VQFN</t>
+  </si>
+  <si>
     <t>Qty</t>
   </si>
   <si>
@@ -1072,6 +1078,9 @@
   </si>
   <si>
     <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 47uF 10V 0805 RoHS</t>
+  </si>
+  <si>
+    <t>IC REG LINEAR POS ADJ 4A 20VQFN</t>
   </si>
 </sst>
 </file>
@@ -1119,7 +1128,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:G102"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.28515625" customWidth="true"/>
@@ -1142,16 +1151,16 @@
         <v>79</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="2">
@@ -1165,16 +1174,16 @@
         <v>80</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="F2">
         <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3">
@@ -1188,16 +1197,16 @@
         <v>81</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F3">
         <v>9</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4">
@@ -1211,16 +1220,16 @@
         <v>82</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F4">
         <v>12</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="5">
@@ -1234,16 +1243,16 @@
         <v>83</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F5">
         <v>187</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6">
@@ -1257,16 +1266,16 @@
         <v>84</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="F6">
         <v>32</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7">
@@ -1280,16 +1289,16 @@
         <v>85</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F7">
         <v>11</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8">
@@ -1303,16 +1312,16 @@
         <v>86</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F8">
         <v>133</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="9">
@@ -1326,16 +1335,16 @@
         <v>87</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F9">
         <v>206</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="10">
@@ -1349,16 +1358,16 @@
         <v>88</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F10">
         <v>86</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="11">
@@ -1372,16 +1381,16 @@
         <v>89</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F11">
         <v>66</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="12">
@@ -1395,16 +1404,16 @@
         <v>90</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F12">
         <v>40</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="13">
@@ -1418,16 +1427,16 @@
         <v>91</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F13">
         <v>8</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="14">
@@ -1441,16 +1450,16 @@
         <v>92</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F14">
         <v>161</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="15">
@@ -1464,16 +1473,16 @@
         <v>93</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F15">
         <v>25</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="16">
@@ -1487,16 +1496,16 @@
         <v>94</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="F16">
         <v>6</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="17">
@@ -1510,16 +1519,16 @@
         <v>95</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F17">
         <v>9</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="18">
@@ -1533,16 +1542,16 @@
         <v>96</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="F18">
         <v>8</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="19">
@@ -1556,16 +1565,16 @@
         <v>97</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F19">
         <v>7</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="20">
@@ -1579,16 +1588,16 @@
         <v>98</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F20">
         <v>9</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="21">
@@ -1602,16 +1611,16 @@
         <v>99</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F21">
         <v>8</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="22">
@@ -1625,16 +1634,16 @@
         <v>100</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F22">
         <v>7</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="23">
@@ -1648,16 +1657,16 @@
         <v>101</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F23">
         <v>1</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="24">
@@ -1671,16 +1680,16 @@
         <v>102</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="F24">
         <v>25</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="25">
@@ -1694,16 +1703,16 @@
         <v>103</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F25">
         <v>4</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="26">
@@ -1717,16 +1726,16 @@
         <v>104</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F26">
         <v>30</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="27">
@@ -1740,16 +1749,16 @@
         <v>105</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="F27">
         <v>2</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="28">
@@ -1763,16 +1772,16 @@
         <v>106</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="F28">
         <v>4</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="29">
@@ -1786,16 +1795,16 @@
         <v>107</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="F29">
         <v>6</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="30">
@@ -1809,16 +1818,16 @@
         <v>108</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F30">
         <v>16</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="31">
@@ -1832,16 +1841,16 @@
         <v>109</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F31">
         <v>4</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="32">
@@ -1855,16 +1864,16 @@
         <v>110</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F32">
         <v>20</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="33">
@@ -1878,16 +1887,16 @@
         <v>111</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="F33">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="34">
@@ -1901,16 +1910,16 @@
         <v>112</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="F34">
         <v>9</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="35">
@@ -1924,16 +1933,16 @@
         <v>113</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F35">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="36">
@@ -1947,16 +1956,16 @@
         <v>114</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="F36">
         <v>22</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="37">
@@ -1970,16 +1979,16 @@
         <v>115</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F37">
         <v>122</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="38">
@@ -1993,16 +2002,16 @@
         <v>116</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F38">
         <v>89</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="39">
@@ -2016,16 +2025,16 @@
         <v>117</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F39">
         <v>95</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="40">
@@ -2039,16 +2048,16 @@
         <v>118</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F40">
         <v>17</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="41">
@@ -2062,16 +2071,16 @@
         <v>119</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F41">
         <v>81</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="42">
@@ -2085,16 +2094,16 @@
         <v>120</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F42">
         <v>87</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="43">
@@ -2108,16 +2117,16 @@
         <v>121</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F43">
         <v>18</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="44">
@@ -2131,16 +2140,16 @@
         <v>122</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F44">
         <v>17</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="45">
@@ -2154,16 +2163,16 @@
         <v>123</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F45">
         <v>65</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="46">
@@ -2177,16 +2186,16 @@
         <v>124</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F46">
         <v>87</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="47">
@@ -2200,16 +2209,16 @@
         <v>125</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F47">
         <v>37</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="48">
@@ -2223,16 +2232,16 @@
         <v>126</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F48">
         <v>248</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="49">
@@ -2246,16 +2255,16 @@
         <v>127</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F49">
         <v>89</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="50">
@@ -2269,16 +2278,16 @@
         <v>128</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F50">
         <v>48</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="51">
@@ -2292,16 +2301,16 @@
         <v>129</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="F51">
         <v>14</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="52">
@@ -2315,16 +2324,16 @@
         <v>130</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F52">
         <v>18</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="53">
@@ -2338,16 +2347,16 @@
         <v>131</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="F53">
         <v>10</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="54">
@@ -2361,16 +2370,16 @@
         <v>132</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="F54">
         <v>10</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="55">
@@ -2384,16 +2393,16 @@
         <v>133</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F55">
         <v>76</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="56">
@@ -2407,16 +2416,16 @@
         <v>134</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F56">
         <v>96</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="57">
@@ -2430,16 +2439,16 @@
         <v>135</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F57">
         <v>6</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="58">
@@ -2453,16 +2462,16 @@
         <v>136</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F58">
         <v>93</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="59">
@@ -2476,16 +2485,16 @@
         <v>137</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F59">
         <v>186</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="60">
@@ -2499,16 +2508,16 @@
         <v>138</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F60">
         <v>100</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="61">
@@ -2522,16 +2531,16 @@
         <v>139</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F61">
         <v>80</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
     </row>
     <row r="62">
@@ -2545,16 +2554,16 @@
         <v>140</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F62">
         <v>86</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="63">
@@ -2568,16 +2577,16 @@
         <v>141</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F63">
         <v>89</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="64">
@@ -2591,16 +2600,16 @@
         <v>142</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F64">
         <v>31</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="65">
@@ -2614,16 +2623,16 @@
         <v>143</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F65">
         <v>44</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="66">
@@ -2637,16 +2646,16 @@
         <v>144</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F66">
         <v>9</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="67">
@@ -2660,16 +2669,16 @@
         <v>145</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F67">
         <v>18</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="68">
@@ -2683,16 +2692,16 @@
         <v>146</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F68">
         <v>51</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="69">
@@ -2706,16 +2715,16 @@
         <v>147</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F69">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
     </row>
     <row r="70">
@@ -2729,16 +2738,16 @@
         <v>148</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F70">
         <v>4</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
     </row>
     <row r="71">
@@ -2752,16 +2761,16 @@
         <v>149</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F71">
         <v>6</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
     </row>
     <row r="72">
@@ -2775,16 +2784,16 @@
         <v>150</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="F72">
         <v>4</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
     </row>
     <row r="73">
@@ -2798,16 +2807,16 @@
         <v>151</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F73">
         <v>4</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
     </row>
     <row r="74">
@@ -2821,16 +2830,16 @@
         <v>152</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F74">
         <v>29</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="75">
@@ -2844,16 +2853,16 @@
         <v>153</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F75">
         <v>2</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
     <row r="76">
@@ -2867,16 +2876,16 @@
         <v>154</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F76">
         <v>9</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="77">
@@ -2890,16 +2899,16 @@
         <v>155</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F77">
         <v>16</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
     <row r="78">
@@ -2913,16 +2922,16 @@
         <v>156</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F78">
         <v>7</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="79">
@@ -2936,16 +2945,16 @@
         <v>157</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F79">
         <v>11</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row r="80">
@@ -2959,16 +2968,16 @@
         <v>158</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F80">
         <v>4</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
     </row>
     <row r="81">
@@ -2982,16 +2991,16 @@
         <v>159</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F81">
         <v>38</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
     </row>
     <row r="82">
@@ -3005,16 +3014,16 @@
         <v>160</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="F82">
         <v>10</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="83">
@@ -3028,16 +3037,16 @@
         <v>161</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F83">
         <v>100</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="84">
@@ -3051,16 +3060,16 @@
         <v>162</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F84">
         <v>50</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="85">
@@ -3074,16 +3083,16 @@
         <v>163</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F85">
         <v>100</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
     </row>
     <row r="86">
@@ -3097,16 +3106,16 @@
         <v>164</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F86">
         <v>50</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="87">
@@ -3120,16 +3129,16 @@
         <v>165</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F87">
         <v>60</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="88">
@@ -3143,16 +3152,16 @@
         <v>166</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="F88">
         <v>20</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
     </row>
     <row r="89">
@@ -3166,16 +3175,16 @@
         <v>167</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F89">
         <v>20</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="90">
@@ -3189,16 +3198,16 @@
         <v>168</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F90">
         <v>100</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="91">
@@ -3212,16 +3221,16 @@
         <v>169</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="F91">
         <v>10</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
     </row>
     <row r="92">
@@ -3235,16 +3244,16 @@
         <v>170</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F92">
         <v>50</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="93">
@@ -3258,16 +3267,16 @@
         <v>171</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F93">
         <v>10</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
     </row>
     <row r="94">
@@ -3281,16 +3290,16 @@
         <v>172</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F94">
         <v>100</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="95">
@@ -3304,16 +3313,16 @@
         <v>173</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F95">
         <v>100</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
     </row>
     <row r="96">
@@ -3327,16 +3336,16 @@
         <v>174</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="F96">
         <v>10</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="97">
@@ -3350,16 +3359,16 @@
         <v>175</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F97">
         <v>100</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
     </row>
     <row r="98">
@@ -3373,16 +3382,16 @@
         <v>176</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F98">
         <v>100</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="99">
@@ -3396,16 +3405,16 @@
         <v>177</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F99">
         <v>20</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="100">
@@ -3419,16 +3428,16 @@
         <v>178</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F100">
         <v>80</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="101">
@@ -3442,16 +3451,39 @@
         <v>179</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="F101">
         <v>20</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>348</v>
+        <v>350</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F102">
+        <v>6</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>355</v>
       </c>
     </row>
   </sheetData>

</xml_diff>